<commit_message>
FINFLUX-2544  Automating Nabkisan Sanity Scenario
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
+++ b/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\finflux_automation_test\Finflux Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
     <sheet name="Summary" sheetId="3" r:id="rId2"/>
     <sheet name="Repayment schedule" sheetId="1" r:id="rId3"/>
     <sheet name="Transactions" sheetId="4" r:id="rId4"/>
+    <sheet name="Modify Transaction1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>#</t>
   </si>
@@ -182,13 +188,28 @@
   </si>
   <si>
     <t>3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH</t>
+  </si>
+  <si>
+    <t>OverDueTillDate</t>
+  </si>
+  <si>
+    <t>clickonsubmit</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>NavigateToLoan</t>
+  </si>
+  <si>
+    <t>navigate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +234,13 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -292,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -335,6 +363,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,6 +374,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,7 +425,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,9 +458,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,6 +510,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -924,7 +991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -1390,4 +1457,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="11">
+        <v>42038</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FINFLUX-2918 Nabkisan 3months compunding and subsidy scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
+++ b/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -341,15 +341,15 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,22 +868,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -974,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -998,49 +998,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22" t="s">
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1447,37 +1447,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="15.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="19">
+      <c r="B1" s="20">
         <v>42038</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "FINFLUX-2918 Nabkisan 3months compunding and subsidy scenarios"
This reverts commit 540834380424860d3668e5e0bbbc2cfd2c8d0577.
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
+++ b/Finflux Automation Excels/Client/3031-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-%INTEREST-Regular-CASH-Newcreateloan1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -341,15 +341,15 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,22 +868,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -974,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -998,49 +998,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18" t="s">
+      <c r="N1" s="22"/>
+      <c r="O1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1447,38 +1447,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="20">
+      <c r="B1" s="19">
         <v>42038</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>